<commit_message>
se mejoro el sistema de busqueda
</commit_message>
<xml_diff>
--- a/plantillas_formatos/Formatos/respaldo/Dulce Daniela Wong Salas/SIMA_SEG_Dulce Daniela Wong Salas.xlsx
+++ b/plantillas_formatos/Formatos/respaldo/Dulce Daniela Wong Salas/SIMA_SEG_Dulce Daniela Wong Salas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mata9585\Desktop\Dany\scripts\Python\V2\LlenadoDeFormatos\plantillas_formatos\Formatos\Dulce Daniela Wong Salas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C9C8FC-EB4B-4861-BAEF-9C4287F1ED22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5677F31D-64F0-4ECB-8DD7-3AC2A3F171D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -707,7 +707,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">  2 de Febrero 2024            </t>
+      <t xml:space="preserve">  14 de Febrero 2024            </t>
     </r>
   </si>
 </sst>
@@ -1259,8 +1259,8 @@
   </sheetPr>
   <dimension ref="A4:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>